<commit_message>
Add | header files
</commit_message>
<xml_diff>
--- a/Game_Design_Document.xlsx
+++ b/Game_Design_Document.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03130BC6-9E86-4EFB-AB2F-6490F0EE5693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="8565" yWindow="2535" windowWidth="11580" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="193">
   <si>
     <t>텍스트 RPG란?</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -804,7 +805,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,11 +1123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1167,7 +1168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1218,11 +1219,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1848,7 +1849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2016,7 +2017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2108,10 +2109,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2345,7 +2346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2433,7 +2434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A15:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -2500,10 +2501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update | 0924 Academy
</commit_message>
<xml_diff>
--- a/Game_Design_Document.xlsx
+++ b/Game_Design_Document.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03130BC6-9E86-4EFB-AB2F-6490F0EE5693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="8565" yWindow="2535" windowWidth="11580" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8565" yWindow="2535" windowWidth="11580" windowHeight="11295" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="194">
   <si>
     <t>텍스트 RPG란?</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -614,10 +613,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>((100/(100+방어)) * 데미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공격 방식에서의 스피드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -626,10 +621,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>50/스피드 : 마다 한번씩 공격한다고 할때…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pq에 넣고 처음 50/스피드를 각자 넣고 해당 시간에서</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -718,18 +709,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5+Lv/2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10+3*lv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5+Lv/4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>법사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -799,13 +782,33 @@
   </si>
   <si>
     <t>*던전에서 몬스터를 잡고 레벨을 올려서 여러 분기로 나뉘어진 상위 클래스로 전직하자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 + lv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200/스피드 : 마다 한번씩 공격한다고 할때…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>((100/(100+방어/2)) * 데미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데미지 * 200 / (200 + 방어)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 + lv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1123,7 +1126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1144,10 +1147,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1157,7 +1160,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1219,11 +1222,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1252,22 +1255,22 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1275,7 +1278,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7">
         <v>60</v>
@@ -1298,7 +1301,7 @@
         <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1306,7 +1309,7 @@
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -1334,7 +1337,7 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -1357,22 +1360,22 @@
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="C13">
-        <v>5.5</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F13">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1380,22 +1383,22 @@
         <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C14">
-        <v>5.0999999999999996</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>6.25</v>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>7.5</v>
+        <v>30</v>
       </c>
       <c r="F14">
-        <v>8.75</v>
+        <v>35</v>
       </c>
       <c r="G14">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1403,10 +1406,10 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F15" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1414,16 +1417,16 @@
         <v>72</v>
       </c>
       <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
         <v>10</v>
       </c>
-      <c r="D16">
-        <v>20</v>
-      </c>
       <c r="E16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1431,16 +1434,16 @@
         <v>73</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1473,7 +1476,7 @@
         <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1484,7 +1487,7 @@
         <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1495,7 +1498,7 @@
         <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1700,6 +1703,11 @@
         <v>142</v>
       </c>
     </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>192</v>
+      </c>
+    </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>143</v>
@@ -1708,7 +1716,7 @@
         <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1758,18 +1766,18 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="H48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1788,7 +1796,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1799,7 +1807,7 @@
         <v>8.33</v>
       </c>
       <c r="E51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1845,11 +1853,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1877,7 +1886,7 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
         <v>82</v>
@@ -1894,7 +1903,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1916,7 +1925,7 @@
         <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F8" t="s">
         <v>105</v>
@@ -1930,7 +1939,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G9" t="s">
         <v>110</v>
@@ -1941,7 +1950,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F10" t="s">
         <v>104</v>
@@ -1955,7 +1964,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G11" t="s">
         <v>111</v>
@@ -1963,7 +1972,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1982,7 +1991,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
         <v>87</v>
@@ -1990,7 +1999,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
         <v>91</v>
@@ -2007,7 +2016,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2109,11 +2118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2244,19 +2253,19 @@
         <v>71</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2264,19 +2273,19 @@
         <v>134</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F13">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2346,7 +2355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2362,17 +2371,17 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2385,16 +2394,16 @@
         <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2402,16 +2411,16 @@
         <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2421,10 +2430,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2434,7 +2443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A15:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -2501,7 +2510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>